<commit_message>
Sorting and demo video
</commit_message>
<xml_diff>
--- a/docs/his_in_one_demo.xlsx
+++ b/docs/his_in_one_demo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oli/Documents/GitHub/grader/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oli/Documents/GitHub/grader/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06387DD-BD1D-8E47-8B93-A625BC0F1697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F59B625-2083-844B-94A6-D8631AA0DDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="500" windowWidth="32000" windowHeight="26900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>14AIN41830 - Stochastik (Prüfung) | Prüfer/-in: Dürr, Oliver | Sommersemester 2025 | Prüfungsperiode 1</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>Leistungsnachweis</t>
-  </si>
-  <si>
-    <t>Klausur</t>
   </si>
   <si>
     <t>49c5f1c3-eb6b-4953-bfac-75b68910e1c1=2,111bd320-814c-4326-9c26-2df41be1f09a=0,f8b01748-fb11-4926-a033-b2aaac6f277c=1,</t>
@@ -581,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -687,10 +684,10 @@
         <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" s="4">
         <v>310000</v>
@@ -717,11 +714,8 @@
       <c r="R6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="T6" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -735,15 +729,17 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="4">
-        <v>310001</v>
-      </c>
-      <c r="G7" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="F7" s="3">
+        <v>300002</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3.7</v>
+      </c>
       <c r="H7" s="4" t="s">
         <v>27</v>
       </c>
@@ -765,11 +761,8 @@
       <c r="R7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S7" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="T7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -783,15 +776,17 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="4">
-        <v>310002</v>
-      </c>
-      <c r="G8" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="F8" s="3">
+        <v>300003</v>
+      </c>
+      <c r="G8" s="3">
+        <v>4</v>
+      </c>
       <c r="H8" s="4" t="s">
         <v>27</v>
       </c>
@@ -813,11 +808,8 @@
       <c r="R8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S8" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="T8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
@@ -831,15 +823,17 @@
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="4">
-        <v>310003</v>
-      </c>
-      <c r="G9" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="F9" s="3">
+        <v>300004</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
       <c r="H9" s="4" t="s">
         <v>27</v>
       </c>
@@ -861,11 +855,8 @@
       <c r="R9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S9" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="T9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -879,13 +870,13 @@
         <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="4">
-        <v>310004</v>
+        <v>310005</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="4" t="s">
@@ -909,11 +900,8 @@
       <c r="R10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S10" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="T10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -927,15 +915,17 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="4">
-        <v>310005</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="F11" s="3">
+        <v>300013</v>
+      </c>
+      <c r="G11" s="3">
+        <v>5</v>
+      </c>
       <c r="H11" s="4" t="s">
         <v>27</v>
       </c>
@@ -957,17 +947,17 @@
       <c r="R11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S11" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="T11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>